<commit_message>
Agenda for 24/2/14 + updated blank DTP Record.xlsx
Agenda for software meeting on 24/2/14 + added test ideas into Blank DTP
Record.xlsx
</commit_message>
<xml_diff>
--- a/Documents/QA/Blank DTP Record.xlsx
+++ b/Documents/QA/Blank DTP Record.xlsx
@@ -12,11 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Test 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Test 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Test 3" sheetId="3" r:id="rId3"/>
-    <sheet name="Test 4" sheetId="4" r:id="rId4"/>
-    <sheet name="Test 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Test Ideas" sheetId="6" r:id="rId1"/>
+    <sheet name="Test 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Test 2" sheetId="2" r:id="rId3"/>
+    <sheet name="Test 3" sheetId="3" r:id="rId4"/>
+    <sheet name="Test 4" sheetId="4" r:id="rId5"/>
+    <sheet name="Test 5" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="19">
   <si>
     <t>Expected Outcome</t>
   </si>
@@ -67,6 +68,24 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>open eclipse</t>
+  </si>
+  <si>
+    <t>eclipse opens</t>
+  </si>
+  <si>
+    <t>Test for mouse click of button to progress through slides</t>
+  </si>
+  <si>
+    <t>Test for audio played (different file types)</t>
+  </si>
+  <si>
+    <t>Test for text objects dispayed on slide (different fonts + sizes + added features)</t>
+  </si>
+  <si>
+    <t>Test for video objects played (also ALL control functions/buttons)</t>
   </si>
 </sst>
 </file>
@@ -396,9 +415,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="76.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -422,6 +481,12 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -474,7 +539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -556,7 +621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -637,7 +702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -719,7 +784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>

</xml_diff>